<commit_message>
Añadidas fechas al excel resultante, versión 4.4
</commit_message>
<xml_diff>
--- a/archivos/maxi-od-3-ACTUALIZADO.xlsx
+++ b/archivos/maxi-od-3-ACTUALIZADO.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F92"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>Nuevo Precio</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Última fecha</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +489,11 @@
           <t>601.598 - (Oscar David)</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -512,6 +522,11 @@
           <t>$ 1.570,16</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -540,6 +555,11 @@
           <t>$ 1.818,10</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2023-12-22 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -568,6 +588,11 @@
           <t>$ 1.363,55</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -596,6 +621,11 @@
           <t>$ 520,58</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -624,6 +654,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2023-12-08 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -652,6 +687,11 @@
           <t>$ 1.570,16</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -680,6 +720,11 @@
           <t>$ 247,85</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -708,6 +753,11 @@
           <t>$ 247,85</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -736,6 +786,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -764,6 +819,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -792,6 +852,11 @@
           <t>$ 991,65</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2023-12-13 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -820,6 +885,11 @@
           <t>$ 2.272,64</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2023-10-20 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -848,6 +918,11 @@
           <t>$ 2.272,64</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2023-11-27 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -876,6 +951,11 @@
           <t>$ 2.272,64</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2023-11-27 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -904,6 +984,11 @@
           <t>$ 3.057,76</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -932,6 +1017,11 @@
           <t>$ 1.115,62</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -960,6 +1050,11 @@
           <t>$ 1.652,81</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -988,6 +1083,11 @@
           <t>$ 991,65</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1016,6 +1116,11 @@
           <t>$ 1.032,97</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1044,6 +1149,11 @@
           <t>$ 1.652,81</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1072,6 +1182,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1100,6 +1215,11 @@
           <t>$ 2.727,19</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1128,6 +1248,11 @@
           <t>$ 1.363,55</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1156,6 +1281,11 @@
           <t>$ 2.396,61</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1184,6 +1314,11 @@
           <t>$ 330,50</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1212,6 +1347,11 @@
           <t>$ 371,82</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1240,6 +1380,11 @@
           <t>$ 371,82</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1268,6 +1413,11 @@
           <t>$ 330,50</t>
         </is>
       </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1296,6 +1446,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1324,6 +1479,11 @@
           <t>$ 2.066,03</t>
         </is>
       </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1352,6 +1512,11 @@
           <t>$ 2.066,03</t>
         </is>
       </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1380,6 +1545,11 @@
           <t>$ 1.266,87</t>
         </is>
       </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1408,6 +1578,11 @@
           <t>$ 1.085,88</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1436,6 +1611,11 @@
           <t>$ 1.221,63</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1464,6 +1644,11 @@
           <t>$ 413,14</t>
         </is>
       </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1492,6 +1677,11 @@
           <t>$ 1.074,29</t>
         </is>
       </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1520,6 +1710,11 @@
           <t>$ 437,93</t>
         </is>
       </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1548,6 +1743,11 @@
           <t>$ 1.239,58</t>
         </is>
       </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1576,6 +1776,11 @@
           <t>$ 1.074,29</t>
         </is>
       </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1604,6 +1809,11 @@
           <t>$ 396,61</t>
         </is>
       </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1632,6 +1842,11 @@
           <t>$ 454,46</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1660,6 +1875,11 @@
           <t>$ 826,36</t>
         </is>
       </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2024-01-12 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1692,6 +1912,11 @@
           <t>1218.962 - (Oscar David)</t>
         </is>
       </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1720,6 +1945,11 @@
           <t>$ 2.479,25</t>
         </is>
       </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2024-01-05 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1748,6 +1978,11 @@
           <t>$ 1.239,59</t>
         </is>
       </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1776,6 +2011,11 @@
           <t>$ 425,54</t>
         </is>
       </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1804,6 +2044,11 @@
           <t>$ 2.479,25</t>
         </is>
       </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1832,6 +2077,11 @@
           <t>$ 1.570,16</t>
         </is>
       </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1860,6 +2110,11 @@
           <t>$ 425,54</t>
         </is>
       </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1888,6 +2143,11 @@
           <t>$ 785,04</t>
         </is>
       </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1916,6 +2176,11 @@
           <t>$ 413,14</t>
         </is>
       </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1944,6 +2209,11 @@
           <t>$ 785,04</t>
         </is>
       </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1972,6 +2242,11 @@
           <t>$ 1.818,09</t>
         </is>
       </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2000,6 +2275,11 @@
           <t>$ 508,18</t>
         </is>
       </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2028,6 +2308,11 @@
           <t>$ 508,18</t>
         </is>
       </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2056,6 +2341,11 @@
           <t>$ 991,65</t>
         </is>
       </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2088,6 +2378,11 @@
           <t>Sin Precio (Ni en Maxiconsumo ni en Oscar David)</t>
         </is>
       </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2120,6 +2415,11 @@
           <t>Sin Precio (Ni en Maxiconsumo ni en Oscar David)</t>
         </is>
       </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2148,6 +2448,11 @@
           <t>$ 413,14</t>
         </is>
       </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2180,6 +2485,11 @@
           <t>Sin Precio (Ni en Maxiconsumo ni en Oscar David)</t>
         </is>
       </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2208,6 +2518,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2236,6 +2551,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2023-12-13 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2264,6 +2584,11 @@
           <t>$ 437,93</t>
         </is>
       </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2292,6 +2617,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2320,6 +2650,11 @@
           <t>$ 1.349,90</t>
         </is>
       </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2348,6 +2683,11 @@
           <t>$ 1.239,90</t>
         </is>
       </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2376,6 +2716,11 @@
           <t>$ 999,90</t>
         </is>
       </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2404,6 +2749,11 @@
           <t>$ 1.299,90</t>
         </is>
       </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2432,6 +2782,11 @@
           <t>$ 1.049,90</t>
         </is>
       </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2460,6 +2815,11 @@
           <t>$ 925,53</t>
         </is>
       </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2488,6 +2848,11 @@
           <t>$ 578,43</t>
         </is>
       </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2024-01-02 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2516,6 +2881,11 @@
           <t>$ 1.818,10</t>
         </is>
       </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2544,6 +2914,11 @@
           <t>$ 2.066,03</t>
         </is>
       </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2572,6 +2947,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2600,6 +2980,11 @@
           <t>$ 950,33</t>
         </is>
       </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2023-11-27 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2628,6 +3013,11 @@
           <t>$ 950,33</t>
         </is>
       </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2023-11-27 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2656,6 +3046,11 @@
           <t>$ 950,33</t>
         </is>
       </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2684,6 +3079,11 @@
           <t>$ 950,33</t>
         </is>
       </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2023-11-27 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2712,6 +3112,11 @@
           <t>$ 950,33</t>
         </is>
       </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2023-11-27 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2740,6 +3145,11 @@
           <t>$ 2.561,90</t>
         </is>
       </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2024-01-23 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2768,6 +3178,11 @@
           <t>$ 2.231,32</t>
         </is>
       </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2796,6 +3211,11 @@
           <t>$ 2.231,32</t>
         </is>
       </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2824,6 +3244,11 @@
           <t>$ 2.231,32</t>
         </is>
       </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>2024-01-16 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2852,6 +3277,11 @@
           <t>$ 909,01</t>
         </is>
       </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>2023-12-21 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2880,6 +3310,11 @@
           <t>$ 2.148,68</t>
         </is>
       </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>2023-12-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2912,6 +3347,11 @@
           <t>3154.974</t>
         </is>
       </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>2023-12-20 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2944,6 +3384,11 @@
           <t>2849.816</t>
         </is>
       </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>2023-12-20 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2976,6 +3421,11 @@
           <t>Sin Precio</t>
         </is>
       </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>2024-01-11 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3004,6 +3454,11 @@
           <t>Sin precio</t>
         </is>
       </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>2024-01-29 00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3030,6 +3485,11 @@
       <c r="F92" t="inlineStr">
         <is>
           <t>Sin precio</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>2024-01-11 00:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadidas funcionalidades varias. Versión 4.6
</commit_message>
<xml_diff>
--- a/archivos/maxi-od-3-ACTUALIZADO.xlsx
+++ b/archivos/maxi-od-3-ACTUALIZADO.xlsx
@@ -479,14 +479,10 @@
           <t>MAXICONSUMO</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1275</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>601.598 - (Oscar David)</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -519,7 +515,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$ 1.570,16</t>
+          <t>$ 1.758,58</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -552,7 +548,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$ 1.818,10</t>
+          <t>$ 2.036,27</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -585,7 +581,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$ 1.363,55</t>
+          <t>$ 1.527,18</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -618,7 +614,7 @@
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$ 520,58</t>
+          <t>$ 629,33</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -684,7 +680,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$ 1.570,16</t>
+          <t>$ 1.758,58</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -717,7 +713,7 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$ 247,85</t>
+          <t>$ 277,59</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -750,7 +746,7 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$ 247,85</t>
+          <t>$ 277,59</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -816,7 +812,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 509,00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -849,7 +845,7 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>$ 991,65</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -882,7 +878,7 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>$ 2.272,64</t>
+          <t>$ 2.545,36</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -915,7 +911,7 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>$ 2.272,64</t>
+          <t>$ 2.545,36</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -948,7 +944,7 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$ 2.272,64</t>
+          <t>$ 2.545,36</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -981,7 +977,7 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$ 3.057,76</t>
+          <t>$ 3.424,69</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1014,7 +1010,7 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$ 1.115,62</t>
+          <t>$ 1.249,49</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1047,7 +1043,7 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1080,7 +1076,7 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>$ 991,65</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1113,7 +1109,7 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>$ 1.032,97</t>
+          <t>$ 925,52</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1146,7 +1142,7 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1212,7 +1208,7 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>$ 2.727,19</t>
+          <t>$ 3.054,45</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1245,7 +1241,7 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>$ 1.363,55</t>
+          <t>$ 1.527,18</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1278,7 +1274,7 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>$ 2.396,61</t>
+          <t>$ 2.684,20</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1311,7 +1307,7 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>$ 330,50</t>
+          <t>$ 370,16</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1344,7 +1340,7 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>$ 371,82</t>
+          <t>$ 416,44</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1377,7 +1373,7 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>$ 371,82</t>
+          <t>$ 416,44</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1410,7 +1406,7 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>$ 330,50</t>
+          <t>$ 370,16</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1476,7 +1472,7 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>$ 2.066,03</t>
+          <t>$ 2.313,95</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1509,7 +1505,7 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>$ 2.066,03</t>
+          <t>$ 2.313,95</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1542,7 +1538,7 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>$ 1.266,87</t>
+          <t>$ 1.418,89</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1575,7 +1571,7 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>$ 1.085,88</t>
+          <t>$ 1.216,19</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1608,7 +1604,7 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>$ 1.221,63</t>
+          <t>$ 1.368,23</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1641,7 +1637,7 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>$ 413,14</t>
+          <t>$ 462,72</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1674,7 +1670,7 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>$ 1.074,29</t>
+          <t>$ 1.203,22</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1707,7 +1703,7 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>$ 437,93</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1740,7 +1736,7 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>$ 1.239,58</t>
+          <t>$ 1.156,94</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1773,7 +1769,7 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>$ 1.074,29</t>
+          <t>$ 1.240,23</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1806,7 +1802,7 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>$ 396,61</t>
+          <t>$ 444,20</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1839,7 +1835,7 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>$ 454,46</t>
+          <t>$ 509,00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -1872,7 +1868,7 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>$ 826,36</t>
+          <t>$ 925,52</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -1902,14 +1898,10 @@
           <t>MAXICONSUMO</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>1248</t>
-        </is>
-      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1218.962 - (Oscar David)</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -1942,7 +1934,7 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>$ 2.479,25</t>
+          <t>$ 3.239,58</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -1975,7 +1967,7 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>$ 1.239,59</t>
+          <t>$ 1.388,34</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2008,7 +2000,7 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>$ 425,54</t>
+          <t>$ 573,79</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2041,7 +2033,7 @@
       <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
-          <t>$ 2.479,25</t>
+          <t>$ 2.776,76</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2074,7 +2066,7 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>$ 1.570,16</t>
+          <t>$ 1.758,58</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2107,7 +2099,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>$ 425,54</t>
+          <t>$ 573,79</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2140,7 +2132,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>$ 785,04</t>
+          <t>$ 768,17</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2173,7 +2165,7 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>$ 413,14</t>
+          <t>$ 462,72</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2206,7 +2198,7 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>$ 785,04</t>
+          <t>$ 879,24</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2239,7 +2231,7 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>$ 1.818,09</t>
+          <t>$ 2.036,26</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2272,7 +2264,7 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>$ 508,18</t>
+          <t>$ 569,16</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2305,7 +2297,7 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>$ 508,18</t>
+          <t>$ 569,16</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2338,7 +2330,7 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>$ 991,65</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2368,14 +2360,10 @@
           <t>MAXICONSUMO</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>451</t>
-        </is>
-      </c>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Sin Precio (Ni en Maxiconsumo ni en Oscar David)</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2405,14 +2393,10 @@
           <t>MAXICONSUMO</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>986</t>
-        </is>
-      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Sin Precio (Ni en Maxiconsumo ni en Oscar David)</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -2445,7 +2429,7 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>$ 413,14</t>
+          <t>$ 462,72</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -2475,14 +2459,10 @@
           <t>MAXICONSUMO</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>446</t>
-        </is>
-      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Sin Precio (Ni en Maxiconsumo ni en Oscar David)</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -2581,7 +2561,7 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>$ 437,93</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -2614,7 +2594,7 @@
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -2647,7 +2627,7 @@
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>$ 1.349,90</t>
+          <t>$ 1.511,89</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -2680,7 +2660,7 @@
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
-          <t>$ 1.239,90</t>
+          <t>$ 1.388,69</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -2713,7 +2693,7 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>$ 999,90</t>
+          <t>$ 1.119,89</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -2746,7 +2726,7 @@
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
-          <t>$ 1.299,90</t>
+          <t>$ 1.455,89</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -2779,7 +2759,7 @@
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
-          <t>$ 1.049,90</t>
+          <t>$ 1.175,89</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -2812,7 +2792,7 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>$ 925,53</t>
+          <t>$ 1.036,59</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -2845,7 +2825,7 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>$ 578,43</t>
+          <t>$ 647,84</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -2878,7 +2858,7 @@
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
-          <t>$ 1.818,10</t>
+          <t>$ 2.036,27</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -2911,7 +2891,7 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>$ 2.066,03</t>
+          <t>$ 2.406,51</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -2977,7 +2957,7 @@
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
-          <t>$ 950,33</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -3010,7 +2990,7 @@
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
-          <t>$ 950,33</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3043,7 +3023,7 @@
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>$ 950,33</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3076,7 +3056,7 @@
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
-          <t>$ 950,33</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -3109,7 +3089,7 @@
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>$ 950,33</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3142,7 +3122,7 @@
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
-          <t>$ 2.561,90</t>
+          <t>$ 2.684,20</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3175,7 +3155,7 @@
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
-          <t>$ 2.231,32</t>
+          <t>$ 2.684,20</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -3208,7 +3188,7 @@
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr">
         <is>
-          <t>$ 2.231,32</t>
+          <t>$ 2.684,20</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3241,7 +3221,7 @@
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
-          <t>$ 2.231,32</t>
+          <t>$ 2.684,20</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -3274,7 +3254,7 @@
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
-          <t>$ 909,01</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3307,7 +3287,7 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>$ 2.148,68</t>
+          <t>$ 2.684,20</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">

</xml_diff>

<commit_message>
Versión 4.7, implementada la búsqueda del archivo de excel desde explorador en reemplazo del sistema de búsqueda en carpeta del directorio del archivo. COmienzo de implementación de adaptación de los precios de los archivos
</commit_message>
<xml_diff>
--- a/archivos/maxi-od-3-ACTUALIZADO.xlsx
+++ b/archivos/maxi-od-3-ACTUALIZADO.xlsx
@@ -482,7 +482,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 453,47</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -548,7 +548,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$ 2.036,27</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -581,7 +581,7 @@
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$ 1.527,18</t>
+          <t>$ 1.480,90</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -779,7 +779,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 444,20</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -845,7 +845,7 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>$ 1.110,65</t>
+          <t>$ 925,52</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -977,7 +977,7 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$ 3.424,69</t>
+          <t>$ 3.054,45</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1109,7 +1109,7 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>$ 925,52</t>
+          <t>$ 1.249,49</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1142,7 +1142,7 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>$ 1.851,15</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1208,7 +1208,7 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>$ 3.054,45</t>
+          <t>$ 3.239,58</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1241,7 +1241,7 @@
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr">
         <is>
-          <t>$ 1.527,18</t>
+          <t>$ 1.295,77</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1274,7 +1274,7 @@
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>$ 2.684,20</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1307,7 +1307,7 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>$ 370,16</t>
+          <t>$ 416,43</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1340,7 +1340,7 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>$ 416,44</t>
+          <t>$ 462,72</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1373,7 +1373,7 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>$ 416,44</t>
+          <t>$ 462,72</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1406,7 +1406,7 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>$ 370,16</t>
+          <t>$ 416,43</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1439,7 +1439,7 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 832,97</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1670,7 +1670,7 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>$ 1.203,22</t>
+          <t>$ 1.388,33</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1703,7 +1703,7 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 499,74</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1736,7 +1736,7 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>$ 1.156,94</t>
+          <t>$ 1.295,77</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1769,7 +1769,7 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>$ 1.240,23</t>
+          <t>$ 990,32</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1934,7 +1934,7 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>$ 3.239,58</t>
+          <t>$ 3.332,13</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2000,7 +2000,7 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>$ 573,79</t>
+          <t>$ 638,58</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2099,7 +2099,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>$ 573,79</t>
+          <t>$ 638,58</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2132,7 +2132,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>$ 768,17</t>
+          <t>$ 879,24</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2264,7 +2264,7 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>$ 569,16</t>
+          <t>$ 601,56</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2297,7 +2297,7 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>$ 569,16</t>
+          <t>$ 601,56</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2561,7 +2561,7 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 509,00</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -2594,7 +2594,7 @@
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 509,00</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -2627,7 +2627,7 @@
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
-          <t>$ 1.511,89</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -2792,7 +2792,7 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>$ 1.036,59</t>
+          <t>$ 1.129,16</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -2825,7 +2825,7 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>$ 647,84</t>
+          <t>$ 740,40</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -2891,7 +2891,7 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>$ 2.406,51</t>
+          <t>$ 2.406,52</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -2957,7 +2957,7 @@
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.064,37</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -2990,7 +2990,7 @@
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.064,37</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3023,7 +3023,7 @@
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.064,37</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3056,7 +3056,7 @@
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.064,37</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -3089,7 +3089,7 @@
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.064,37</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3122,7 +3122,7 @@
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
-          <t>$ 2.684,20</t>
+          <t>$ 2.961,88</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">

</xml_diff>

<commit_message>
Implementada la apertura manual de sesiones por ID de sesión. Valuador incorporado y funcional. Taskbar funcional.
</commit_message>
<xml_diff>
--- a/archivos/maxi-od-3-ACTUALIZADO.xlsx
+++ b/archivos/maxi-od-3-ACTUALIZADO.xlsx
@@ -482,7 +482,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$ 454,46</t>
+          <t>$ 601,56</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -515,7 +515,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -548,7 +548,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 1.018,14</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -655,7 +655,7 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$ 1.487,52</t>
+          <t>$ 1.758,58</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -688,7 +688,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$ 561,90</t>
+          <t>$ 629,33</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -758,7 +758,7 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 481,23</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -791,7 +791,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -824,7 +824,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>$ 272,64</t>
+          <t>$ 305,36</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -857,7 +857,7 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>$ 272,64</t>
+          <t>$ 305,36</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -890,7 +890,7 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>$ 437,93</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -923,7 +923,7 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>$ 454,46</t>
+          <t>$ 555,28</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -956,7 +956,7 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$ 909,00</t>
+          <t>$ 1.018,08</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -989,7 +989,7 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$ 2.190,00</t>
+          <t>$ 2.452,80</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1022,7 +1022,7 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$ 2.190,00</t>
+          <t>$ 2.452,80</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1055,7 +1055,7 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>$ 2.190,00</t>
+          <t>$ 2.452,80</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1088,7 +1088,7 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>$ 2.479,26</t>
+          <t>$ 3.239,58</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1121,7 +1121,7 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>$ 1.115,62</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1154,7 +1154,7 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 1.758,58</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1187,7 +1187,7 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>$ 991,65</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1220,7 +1220,7 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 1.064,37</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1319,7 +1319,7 @@
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Sin Precio</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1352,7 +1352,7 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>$ 2.975,12</t>
+          <t>$ 3.332,13</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1385,7 +1385,7 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>$ 1.239,59</t>
+          <t>$ 1.666,02</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1418,7 +1418,7 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>$ 2.644,54</t>
+          <t>$ 2.961,88</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1451,7 +1451,7 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>$ 396,61</t>
+          <t>$ 407,18</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1484,7 +1484,7 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>$ 437,93</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1517,7 +1517,7 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>$ 371,82</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1550,7 +1550,7 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>$ 330,50</t>
+          <t>$ 407,18</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1583,7 +1583,7 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 832,97</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1616,7 +1616,7 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>$ 2.066,03</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1649,7 +1649,7 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>$ 2.066,03</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1682,7 +1682,7 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>$ 1.429,77</t>
+          <t>$ 1.601,34</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1715,7 +1715,7 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>$ 1.239,73</t>
+          <t>$ 1.388,50</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1748,7 +1748,7 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>$ 1.330,23</t>
+          <t>$ 1.489,86</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1781,7 +1781,7 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>$ 437,93</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1814,7 +1814,7 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>$ 1.156,94</t>
+          <t>$ 1.295,77</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1847,7 +1847,7 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>$ 454,46</t>
+          <t>$ 509,00</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -1880,7 +1880,7 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 1.295,77</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -1913,7 +1913,7 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>$ 1.016,44</t>
+          <t>$ 1.138,41</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -1946,7 +1946,7 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>$ 437,93</t>
+          <t>$ 490,48</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -1979,7 +1979,7 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>$ 495,79</t>
+          <t>$ 555,28</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2012,7 +2012,7 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>$ 909,00</t>
+          <t>$ 1.018,08</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2111,7 +2111,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Sin precio</t>
+          <t>$ 1.203,22</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2144,7 +2144,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>$ 578,43</t>
+          <t>$ 740,40</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2177,7 +2177,7 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>$ 2.661,07</t>
+          <t>$ 2.980,40</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2210,7 +2210,7 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>$ 1.652,81</t>
+          <t>$ 1.851,15</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2243,7 +2243,7 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>$ 578,43</t>
+          <t>$ 740,40</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2276,7 +2276,7 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>$ 826,36</t>
+          <t>$ 786,69</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2309,7 +2309,7 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>$ 454,46</t>
+          <t>$ 509,00</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2342,7 +2342,7 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>$ 842,89</t>
+          <t>$ 944,04</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2375,7 +2375,7 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>$ 1.983,38</t>
+          <t>$ 2.221,39</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2408,7 +2408,7 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>$ 578,43</t>
+          <t>$ 647,84</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -2441,7 +2441,7 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>$ 578,43</t>
+          <t>$ 647,84</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -2474,7 +2474,7 @@
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>$ 991,65</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -2573,7 +2573,7 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>$ 413,14</t>
+          <t>$ 481,22</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -2705,7 +2705,7 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>$ 479,26</t>
+          <t>$ 536,77</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -2738,7 +2738,7 @@
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
-          <t>$ 479,26</t>
+          <t>$ 536,77</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -2804,7 +2804,7 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>$ 1.239,90</t>
+          <t>$ 1.388,69</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -2837,7 +2837,7 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>$ 999,90</t>
+          <t>$ 1.119,89</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -2870,7 +2870,7 @@
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
-          <t>$ 1.299,90</t>
+          <t>$ 1.455,89</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -2903,7 +2903,7 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>$ 1.049,90</t>
+          <t>$ 1.175,89</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -2936,7 +2936,7 @@
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
-          <t>$ 1.074,29</t>
+          <t>$ 1.203,20</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -2969,7 +2969,7 @@
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
-          <t>$ 702,39</t>
+          <t>$ 786,68</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -3002,7 +3002,7 @@
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
-          <t>$ 1.983,39</t>
+          <t>$ 2.036,27</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3035,7 +3035,7 @@
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>$ 2.272,64</t>
+          <t>$ 2.545,36</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3068,7 +3068,7 @@
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
-          <t>$ 1.322,23</t>
+          <t>$ 1.480,90</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -3101,7 +3101,7 @@
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>$ 933,80</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3134,7 +3134,7 @@
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
-          <t>$ 933,80</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3167,7 +3167,7 @@
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
-          <t>$ 933,80</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -3200,7 +3200,7 @@
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr">
         <is>
-          <t>$ 933,80</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3233,7 +3233,7 @@
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
-          <t>$ 933,80</t>
+          <t>$ 1.156,93</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -3266,7 +3266,7 @@
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
-          <t>$ 2.479,26</t>
+          <t>$ 2.776,77</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3299,7 +3299,7 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>$ 2.768,51</t>
+          <t>$ 3.100,73</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -3332,7 +3332,7 @@
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Sin Precio</t>
+          <t>Sin precio</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -3365,7 +3365,7 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
-          <t>$ 2.768,51</t>
+          <t>$ 3.100,73</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -3398,7 +3398,7 @@
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
-          <t>$ 2.768,51</t>
+          <t>$ 3.100,73</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -3431,7 +3431,7 @@
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
-          <t>$ 991,65</t>
+          <t>$ 1.110,65</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -3464,7 +3464,7 @@
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr">
         <is>
-          <t>$ 2.231,32</t>
+          <t>$ 2.776,77</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">

</xml_diff>

<commit_message>
Lector actualizado. Versión funcional. Único cambio pendiente: Implementación de búsqueda doble
</commit_message>
<xml_diff>
--- a/archivos/maxi-od-3-ACTUALIZADO.xlsx
+++ b/archivos/maxi-od-3-ACTUALIZADO.xlsx
@@ -482,7 +482,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$ 601,56</t>
+          <t>$ 537,11</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -515,7 +515,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$ 1.851,15</t>
+          <t>$ 1.652,81</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -548,7 +548,7 @@
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$ 1.018,14</t>
+          <t>$ 909,05</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -655,7 +655,7 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$ 1.758,58</t>
+          <t>$ 1.570,16</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -688,7 +688,7 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$ 629,33</t>
+          <t>$ 561,90</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -758,7 +758,7 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$ 481,23</t>
+          <t>$ 429,67</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -791,7 +791,7 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>$ 1.851,15</t>
+          <t>$ 1.652,81</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -824,7 +824,7 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>$ 305,36</t>
+          <t>$ 272,64</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -857,7 +857,7 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>$ 305,36</t>
+          <t>$ 272,64</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -890,7 +890,7 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 437,93</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -923,7 +923,7 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>$ 555,28</t>
+          <t>$ 495,79</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -956,7 +956,7 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$ 1.018,08</t>
+          <t>$ 909,00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -989,7 +989,7 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$ 2.452,80</t>
+          <t>$ 2.190,00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1022,7 +1022,7 @@
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$ 2.452,80</t>
+          <t>$ 2.190,00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1055,7 +1055,7 @@
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>$ 2.452,80</t>
+          <t>$ 2.190,00</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1088,7 +1088,7 @@
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>$ 3.239,58</t>
+          <t>$ 2.892,48</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1121,7 +1121,7 @@
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>$ 1.110,65</t>
+          <t>$ 991,65</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1154,7 +1154,7 @@
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>$ 1.758,58</t>
+          <t>$ 1.570,16</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1187,7 +1187,7 @@
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>$ 1.110,65</t>
+          <t>$ 991,65</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1220,7 +1220,7 @@
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>$ 1.064,37</t>
+          <t>$ 950,33</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1352,7 +1352,7 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>$ 3.332,13</t>
+          <t>$ 2.975,12</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1385,7 +1385,7 @@
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>$ 1.666,02</t>
+          <t>$ 1.487,52</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1418,7 +1418,7 @@
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>$ 2.961,88</t>
+          <t>$ 2.644,54</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1451,7 +1451,7 @@
       <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>$ 407,18</t>
+          <t>$ 363,55</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1484,7 +1484,7 @@
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 437,93</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1517,7 +1517,7 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 437,93</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1550,7 +1550,7 @@
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>$ 407,18</t>
+          <t>$ 363,55</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1583,7 +1583,7 @@
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>$ 832,97</t>
+          <t>$ 743,72</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1616,7 +1616,7 @@
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>$ 1.851,15</t>
+          <t>$ 1.652,81</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1649,7 +1649,7 @@
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>$ 1.851,15</t>
+          <t>$ 1.652,81</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1682,7 +1682,7 @@
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>$ 1.601,34</t>
+          <t>$ 1.429,77</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1715,7 +1715,7 @@
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr">
         <is>
-          <t>$ 1.388,50</t>
+          <t>$ 1.239,73</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1748,7 +1748,7 @@
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>$ 1.489,86</t>
+          <t>$ 1.330,23</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1781,7 +1781,7 @@
       <c r="E41" t="inlineStr"/>
       <c r="F41" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 437,93</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1814,7 +1814,7 @@
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>$ 1.295,77</t>
+          <t>$ 1.156,94</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1847,7 +1847,7 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" t="inlineStr">
         <is>
-          <t>$ 509,00</t>
+          <t>$ 454,46</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -1880,7 +1880,7 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>$ 1.295,77</t>
+          <t>$ 1.156,94</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -1913,7 +1913,7 @@
       <c r="E45" t="inlineStr"/>
       <c r="F45" t="inlineStr">
         <is>
-          <t>$ 1.138,41</t>
+          <t>$ 1.016,44</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -1946,7 +1946,7 @@
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>$ 490,48</t>
+          <t>$ 437,93</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -1979,7 +1979,7 @@
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>$ 555,28</t>
+          <t>$ 495,79</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2012,7 +2012,7 @@
       <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>$ 1.018,08</t>
+          <t>$ 909,00</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2111,7 +2111,7 @@
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>$ 1.203,22</t>
+          <t>$ 1.074,30</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2144,7 +2144,7 @@
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>$ 740,40</t>
+          <t>$ 661,07</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2177,7 +2177,7 @@
       <c r="E53" t="inlineStr"/>
       <c r="F53" t="inlineStr">
         <is>
-          <t>$ 2.980,40</t>
+          <t>$ 2.661,07</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2210,7 +2210,7 @@
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
-          <t>$ 1.851,15</t>
+          <t>$ 1.652,81</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2243,7 +2243,7 @@
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>$ 740,40</t>
+          <t>$ 661,07</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2276,7 +2276,7 @@
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>$ 786,69</t>
+          <t>$ 702,40</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2309,7 +2309,7 @@
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>$ 509,00</t>
+          <t>$ 454,46</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2342,7 +2342,7 @@
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>$ 944,04</t>
+          <t>$ 842,89</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2375,7 +2375,7 @@
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>$ 2.221,39</t>
+          <t>$ 1.983,38</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2408,7 +2408,7 @@
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>$ 647,84</t>
+          <t>$ 578,43</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -2441,7 +2441,7 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>$ 647,84</t>
+          <t>$ 578,43</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -2474,7 +2474,7 @@
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
-          <t>$ 1.110,65</t>
+          <t>$ 991,65</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -2573,7 +2573,7 @@
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
-          <t>$ 481,22</t>
+          <t>$ 429,66</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -2705,7 +2705,7 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
-          <t>$ 536,77</t>
+          <t>$ 479,26</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -2738,7 +2738,7 @@
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
-          <t>$ 536,77</t>
+          <t>$ 479,26</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -2804,7 +2804,7 @@
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
-          <t>$ 1.388,69</t>
+          <t>$ 1.239,90</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -2837,7 +2837,7 @@
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
-          <t>$ 1.119,89</t>
+          <t>$ 999,90</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
@@ -2870,7 +2870,7 @@
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
-          <t>$ 1.455,89</t>
+          <t>$ 1.299,90</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -2903,7 +2903,7 @@
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
-          <t>$ 1.175,89</t>
+          <t>$ 1.049,90</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -2936,7 +2936,7 @@
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
-          <t>$ 1.203,20</t>
+          <t>$ 1.074,29</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -2969,7 +2969,7 @@
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
-          <t>$ 786,68</t>
+          <t>$ 702,39</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -3002,7 +3002,7 @@
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
-          <t>$ 2.036,27</t>
+          <t>$ 1.818,10</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3035,7 +3035,7 @@
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
-          <t>$ 2.545,36</t>
+          <t>$ 2.272,64</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3068,7 +3068,7 @@
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
-          <t>$ 1.480,90</t>
+          <t>$ 1.322,23</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -3101,7 +3101,7 @@
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.032,97</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3134,7 +3134,7 @@
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.032,97</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3167,7 +3167,7 @@
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.032,97</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -3200,7 +3200,7 @@
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.032,97</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3233,7 +3233,7 @@
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
-          <t>$ 1.156,93</t>
+          <t>$ 1.032,97</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -3266,7 +3266,7 @@
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
-          <t>$ 2.776,77</t>
+          <t>$ 2.479,26</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3299,7 +3299,7 @@
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr">
         <is>
-          <t>$ 3.100,73</t>
+          <t>$ 2.768,51</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -3365,7 +3365,7 @@
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>
-          <t>$ 3.100,73</t>
+          <t>$ 2.768,51</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -3398,7 +3398,7 @@
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
         <is>
-          <t>$ 3.100,73</t>
+          <t>$ 2.768,51</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -3431,7 +3431,7 @@
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
         <is>
-          <t>$ 1.110,65</t>
+          <t>$ 991,65</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -3464,7 +3464,7 @@
       <c r="E92" t="inlineStr"/>
       <c r="F92" t="inlineStr">
         <is>
-          <t>$ 2.776,77</t>
+          <t>$ 2.479,26</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">

</xml_diff>